<commit_message>
Fixed toString method for Scoop for multiple toppings.
</commit_message>
<xml_diff>
--- a/P05/Scrum.xlsx
+++ b/P05/Scrum.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="1"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -26,7 +26,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="186">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="373" uniqueCount="189">
   <si>
     <t xml:space="preserve">Product Name:</t>
   </si>
@@ -40,6 +40,9 @@
     <t xml:space="preserve">Team ID:</t>
   </si>
   <si>
+    <t xml:space="preserve">Of MICE and Man</t>
+  </si>
+  <si>
     <t xml:space="preserve">Team Member Name</t>
   </si>
   <si>
@@ -52,6 +55,12 @@
     <t xml:space="preserve">Required</t>
   </si>
   <si>
+    <t xml:space="preserve">Ethan Sprinkle</t>
+  </si>
+  <si>
+    <t xml:space="preserve">ES</t>
+  </si>
+  <si>
     <t xml:space="preserve">Sprint #</t>
   </si>
   <si>
@@ -146,9 +155,6 @@
   </si>
   <si>
     <t xml:space="preserve">MX</t>
-  </si>
-  <si>
-    <t xml:space="preserve">In Test</t>
   </si>
   <si>
     <t xml:space="preserve">Create a “mix in” request including amount to mix in</t>
@@ -580,6 +586,7 @@
         <color rgb="FF000000"/>
         <rFont val="Arial"/>
         <family val="2"/>
+        <charset val="1"/>
       </rPr>
       <t xml:space="preserve">and Item Superclass</t>
     </r>
@@ -591,23 +598,10 @@
     <t xml:space="preserve">In Work</t>
   </si>
   <si>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-        <charset val="1"/>
-      </rPr>
-      <t xml:space="preserve">Scoop Class created. </t>
-    </r>
-    <r>
-      <rPr>
-        <sz val="10"/>
-        <rFont val="Arial"/>
-        <family val="2"/>
-      </rPr>
-      <t xml:space="preserve">Debugging toString Method for multiple MixIns.</t>
-    </r>
+    <t xml:space="preserve">Scoop Class created. Debugging toString Method for multiple MixIns.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Fixed toString method in Scoop to print multiple toppings.</t>
   </si>
   <si>
     <t xml:space="preserve">--&gt; Add tasks to complete each feature for this sprint</t>
@@ -629,7 +623,7 @@
     <numFmt numFmtId="166" formatCode="mmm\ dd"/>
     <numFmt numFmtId="167" formatCode="mm/dd/yy\ hh:mm\ AM/PM"/>
   </numFmts>
-  <fonts count="18">
+  <fonts count="17">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -743,11 +737,6 @@
     <font>
       <sz val="9"/>
       <color rgb="FF000000"/>
-      <name val="Arial"/>
-      <family val="2"/>
-    </font>
-    <font>
-      <sz val="10"/>
       <name val="Arial"/>
       <family val="2"/>
     </font>
@@ -1041,7 +1030,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1087,10 +1076,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0822405395279131"/>
-          <c:y val="0.161875945537065"/>
-          <c:w val="0.884351192706382"/>
-          <c:h val="0.63565305093293"/>
+          <c:x val="0.0822456753887466"/>
+          <c:y val="0.161896356071113"/>
+          <c:w val="0.884281521263973"/>
+          <c:h val="0.635607111335267"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1177,33 +1166,33 @@
                   <c:v>39</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>37</c:v>
+                  <c:v>35</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="49046774"/>
-        <c:axId val="27834190"/>
+        <c:axId val="12571629"/>
+        <c:axId val="98322254"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="49046774"/>
+        <c:axId val="12571629"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1270,12 +1259,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27834190"/>
+        <c:crossAx val="98322254"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="27834190"/>
+        <c:axId val="98322254"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1350,7 +1339,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="49046774"/>
+        <c:crossAx val="12571629"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1370,14 +1359,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1487,10 +1476,10 @@
                   <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>2</c:v>
+                  <c:v>0</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1505,11 +1494,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="59853049"/>
-        <c:axId val="47434210"/>
+        <c:axId val="75376761"/>
+        <c:axId val="1498183"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="59853049"/>
+        <c:axId val="75376761"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1574,7 +1563,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="47434210"/>
+        <c:crossAx val="1498183"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1582,7 +1571,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="47434210"/>
+        <c:axId val="1498183"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1656,7 +1645,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="59853049"/>
+        <c:crossAx val="75376761"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1676,14 +1665,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1811,11 +1800,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="28941477"/>
-        <c:axId val="43434615"/>
+        <c:axId val="43272625"/>
+        <c:axId val="89107661"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="28941477"/>
+        <c:axId val="43272625"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1880,7 +1869,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43434615"/>
+        <c:crossAx val="89107661"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1888,7 +1877,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="43434615"/>
+        <c:axId val="89107661"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1962,7 +1951,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="28941477"/>
+        <c:crossAx val="43272625"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1982,14 +1971,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2117,11 +2106,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="5108432"/>
-        <c:axId val="61579846"/>
+        <c:axId val="44556670"/>
+        <c:axId val="29980569"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="5108432"/>
+        <c:axId val="44556670"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2186,7 +2175,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="61579846"/>
+        <c:crossAx val="29980569"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2194,7 +2183,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="61579846"/>
+        <c:axId val="29980569"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2268,7 +2257,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="5108432"/>
+        <c:crossAx val="44556670"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2288,14 +2277,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2423,11 +2412,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="82733410"/>
-        <c:axId val="23569597"/>
+        <c:axId val="27674405"/>
+        <c:axId val="74548752"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82733410"/>
+        <c:axId val="27674405"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2492,7 +2481,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="23569597"/>
+        <c:crossAx val="74548752"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2500,7 +2489,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="23569597"/>
+        <c:axId val="74548752"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2574,7 +2563,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82733410"/>
+        <c:crossAx val="27674405"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2594,14 +2583,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2729,11 +2718,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="18464144"/>
-        <c:axId val="36597349"/>
+        <c:axId val="57129197"/>
+        <c:axId val="22977046"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="18464144"/>
+        <c:axId val="57129197"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2798,7 +2787,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="36597349"/>
+        <c:crossAx val="22977046"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2806,7 +2795,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="36597349"/>
+        <c:axId val="22977046"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2880,7 +2869,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="18464144"/>
+        <c:crossAx val="57129197"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2900,14 +2889,14 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3035,11 +3024,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="8426005"/>
-        <c:axId val="11657437"/>
+        <c:axId val="82518941"/>
+        <c:axId val="77650874"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="8426005"/>
+        <c:axId val="82518941"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3104,7 +3093,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="11657437"/>
+        <c:crossAx val="77650874"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3112,7 +3101,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="11657437"/>
+        <c:axId val="77650874"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3186,7 +3175,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="8426005"/>
+        <c:crossAx val="82518941"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3206,7 +3195,7 @@
     <a:solidFill>
       <a:srgbClr val="ffffff"/>
     </a:solidFill>
-    <a:ln>
+    <a:ln w="9360">
       <a:noFill/>
     </a:ln>
   </c:spPr>
@@ -3224,9 +3213,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3201840</xdr:colOff>
+      <xdr:colOff>3201480</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>120240</xdr:rowOff>
+      <xdr:rowOff>119880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3234,8 +3223,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9117720" y="267840"/>
-        <a:ext cx="5764680" cy="2855160"/>
+        <a:off x="9115920" y="267840"/>
+        <a:ext cx="5764320" cy="2854800"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3259,9 +3248,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3269,8 +3258,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3294,9 +3283,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3304,8 +3293,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3329,9 +3318,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3339,8 +3328,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3364,9 +3353,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3374,8 +3363,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3399,9 +3388,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3409,8 +3398,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3434,9 +3423,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518400</xdr:colOff>
+      <xdr:colOff>518040</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129600</xdr:rowOff>
+      <xdr:rowOff>129240</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3444,8 +3433,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4088880" y="446400"/>
-        <a:ext cx="3747240" cy="1847880"/>
+        <a:off x="4090680" y="446400"/>
+        <a:ext cx="3747600" cy="1847520"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3466,8 +3455,8 @@
   </sheetPr>
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A10" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="K27" activeCellId="0" sqref="K27"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3475,11 +3464,11 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="1" width="13.7"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="2" min="2" style="1" width="10.99"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.57"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.42"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.71"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.58"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="45.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="10" min="10" style="1" width="39.14"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="11" min="11" style="1" width="53.71"/>
@@ -3507,7 +3496,9 @@
       <c r="A2" s="1" t="s">
         <v>3</v>
       </c>
-      <c r="B2" s="6"/>
+      <c r="B2" s="6" t="s">
+        <v>4</v>
+      </c>
       <c r="C2" s="6"/>
       <c r="D2" s="6"/>
       <c r="E2" s="6"/>
@@ -3532,7 +3523,7 @@
     <row r="4" s="5" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="1"/>
       <c r="B4" s="3" t="s">
-        <v>4</v>
+        <v>5</v>
       </c>
       <c r="C4" s="3"/>
       <c r="D4" s="3"/>
@@ -3540,25 +3531,31 @@
       <c r="F4" s="3"/>
       <c r="G4" s="3"/>
       <c r="H4" s="3" t="s">
-        <v>5</v>
+        <v>6</v>
       </c>
       <c r="I4" s="3" t="s">
-        <v>6</v>
+        <v>7</v>
       </c>
       <c r="J4" s="3"/>
     </row>
     <row r="5" s="5" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A5" s="1" t="s">
-        <v>7</v>
-      </c>
-      <c r="B5" s="7"/>
+        <v>8</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>9</v>
+      </c>
       <c r="C5" s="7"/>
       <c r="D5" s="7"/>
       <c r="E5" s="7"/>
       <c r="F5" s="7"/>
       <c r="G5" s="7"/>
-      <c r="H5" s="7"/>
-      <c r="I5" s="7"/>
+      <c r="H5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="I5" s="7" t="n">
+        <v>1002002357</v>
+      </c>
       <c r="J5" s="3"/>
     </row>
     <row r="6" s="5" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -3578,19 +3575,19 @@
     </row>
     <row r="11" s="5" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="8" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B11" s="9" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C11" s="10" t="s">
-        <v>10</v>
+        <v>13</v>
       </c>
       <c r="D11" s="10"/>
       <c r="E11" s="3"/>
       <c r="F11" s="3"/>
       <c r="G11" s="3" t="s">
-        <v>11</v>
+        <v>14</v>
       </c>
       <c r="H11" s="3"/>
       <c r="I11" s="3"/>
@@ -3608,10 +3605,10 @@
       <c r="D12" s="10"/>
       <c r="E12" s="3"/>
       <c r="F12" s="12" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="G12" s="3" t="s">
-        <v>13</v>
+        <v>16</v>
       </c>
       <c r="H12" s="3"/>
       <c r="I12" s="3"/>
@@ -3623,11 +3620,11 @@
       </c>
       <c r="B13" s="3" t="n">
         <f aca="false">B12-C13</f>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C13" s="10" t="n">
         <f aca="false">COUNTIF(G$24:G$107,"Finished in Sprint 1")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D13" s="10"/>
       <c r="E13" s="3"/>
@@ -3635,7 +3632,7 @@
         <v>1</v>
       </c>
       <c r="G13" s="3" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="H13" s="3"/>
       <c r="I13" s="3"/>
@@ -3647,7 +3644,7 @@
       </c>
       <c r="B14" s="3" t="n">
         <f aca="false">B13-C14</f>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C14" s="10" t="n">
         <f aca="false">COUNTIF(G$24:G$107,"Finished in Sprint 2")</f>
@@ -3659,7 +3656,7 @@
         <v>2</v>
       </c>
       <c r="G14" s="3" t="s">
-        <v>15</v>
+        <v>18</v>
       </c>
       <c r="H14" s="3"/>
       <c r="I14" s="3"/>
@@ -3671,7 +3668,7 @@
       </c>
       <c r="B15" s="3" t="n">
         <f aca="false">B14-C15</f>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C15" s="10" t="n">
         <f aca="false">COUNTIF(G$24:G$107,"Finished in Sprint 3")</f>
@@ -3683,7 +3680,7 @@
         <v>3</v>
       </c>
       <c r="G15" s="3" t="s">
-        <v>16</v>
+        <v>19</v>
       </c>
       <c r="H15" s="3"/>
       <c r="I15" s="3"/>
@@ -3695,7 +3692,7 @@
       </c>
       <c r="B16" s="3" t="n">
         <f aca="false">B15-C16</f>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C16" s="10" t="n">
         <f aca="false">COUNTIF(G$24:G$107,"Finished in Sprint 4")</f>
@@ -3715,7 +3712,7 @@
       </c>
       <c r="B17" s="3" t="n">
         <f aca="false">B16-C17</f>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C17" s="10" t="n">
         <f aca="false">COUNTIF(G$24:G$107,"Finished in Sprint 5")</f>
@@ -3735,7 +3732,7 @@
       </c>
       <c r="B18" s="3" t="n">
         <f aca="false">B17-C18</f>
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="C18" s="10" t="n">
         <f aca="false">COUNTIF(G$24:G$107,"Finished in Sprint 6")</f>
@@ -3770,7 +3767,7 @@
       <c r="F20" s="3"/>
       <c r="G20" s="3"/>
       <c r="H20" s="13" t="s">
-        <v>17</v>
+        <v>20</v>
       </c>
       <c r="I20" s="3"/>
       <c r="J20" s="3"/>
@@ -3784,7 +3781,7 @@
       <c r="F21" s="3"/>
       <c r="G21" s="3"/>
       <c r="H21" s="3" t="s">
-        <v>18</v>
+        <v>21</v>
       </c>
       <c r="I21" s="3"/>
       <c r="J21" s="3"/>
@@ -3796,7 +3793,7 @@
       <c r="D22" s="14"/>
       <c r="E22" s="14"/>
       <c r="F22" s="15" t="s">
-        <v>19</v>
+        <v>22</v>
       </c>
       <c r="G22" s="15"/>
       <c r="H22" s="14"/>
@@ -3805,42 +3802,42 @@
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="16" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="B23" s="16" t="s">
-        <v>21</v>
+        <v>24</v>
       </c>
       <c r="C23" s="16" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="D23" s="16" t="s">
-        <v>22</v>
+        <v>25</v>
       </c>
       <c r="E23" s="16" t="s">
-        <v>23</v>
+        <v>26</v>
       </c>
       <c r="F23" s="16" t="s">
-        <v>24</v>
+        <v>27</v>
       </c>
       <c r="G23" s="16" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="H23" s="16" t="s">
-        <v>26</v>
+        <v>29</v>
       </c>
       <c r="I23" s="16" t="s">
-        <v>27</v>
+        <v>30</v>
       </c>
       <c r="J23" s="16" t="s">
-        <v>28</v>
+        <v>31</v>
       </c>
       <c r="K23" s="16" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="24" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A24" s="1" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="B24" s="11" t="n">
         <v>1</v>
@@ -3856,24 +3853,24 @@
         <v>1</v>
       </c>
       <c r="G24" s="18" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H24" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I24" s="19" t="s">
-        <v>33</v>
+        <v>36</v>
       </c>
       <c r="J24" s="19" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K24" s="19" t="s">
-        <v>35</v>
+        <v>38</v>
       </c>
     </row>
     <row r="25" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A25" s="1" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="B25" s="11" t="n">
         <v>2</v>
@@ -3889,24 +3886,24 @@
         <v>1</v>
       </c>
       <c r="G25" s="18" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H25" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I25" s="19" t="s">
-        <v>37</v>
+        <v>40</v>
       </c>
       <c r="J25" s="19" t="s">
+        <v>41</v>
+      </c>
+      <c r="K25" s="19" t="s">
         <v>38</v>
-      </c>
-      <c r="K25" s="19" t="s">
-        <v>35</v>
       </c>
     </row>
     <row r="26" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A26" s="1" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="B26" s="11" t="n">
         <v>3</v>
@@ -3922,24 +3919,24 @@
         <v>1</v>
       </c>
       <c r="G26" s="18" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H26" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I26" s="19" t="s">
-        <v>41</v>
+        <v>43</v>
       </c>
       <c r="J26" s="19" t="s">
-        <v>42</v>
+        <v>44</v>
       </c>
       <c r="K26" s="19" t="s">
-        <v>43</v>
+        <v>45</v>
       </c>
     </row>
     <row r="27" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A27" s="1" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="B27" s="11" t="n">
         <v>4</v>
@@ -3955,24 +3952,24 @@
         <v>1</v>
       </c>
       <c r="G27" s="18" t="s">
-        <v>40</v>
+        <v>34</v>
       </c>
       <c r="H27" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I27" s="19" t="s">
-        <v>45</v>
+        <v>47</v>
       </c>
       <c r="J27" s="19" t="s">
-        <v>46</v>
+        <v>48</v>
       </c>
       <c r="K27" s="19" t="s">
-        <v>47</v>
+        <v>49</v>
       </c>
     </row>
     <row r="28" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A28" s="1" t="s">
-        <v>48</v>
+        <v>50</v>
       </c>
       <c r="B28" s="11" t="n">
         <v>5</v>
@@ -3987,21 +3984,21 @@
       <c r="F28" s="17"/>
       <c r="G28" s="18"/>
       <c r="H28" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I28" s="19" t="s">
-        <v>49</v>
+        <v>51</v>
       </c>
       <c r="J28" s="19" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K28" s="19" t="s">
-        <v>51</v>
+        <v>53</v>
       </c>
     </row>
     <row r="29" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A29" s="1" t="s">
-        <v>52</v>
+        <v>54</v>
       </c>
       <c r="B29" s="11" t="n">
         <v>6</v>
@@ -4016,21 +4013,21 @@
       <c r="F29" s="17"/>
       <c r="G29" s="18"/>
       <c r="H29" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I29" s="19" t="s">
-        <v>53</v>
+        <v>55</v>
       </c>
       <c r="J29" s="19" t="s">
-        <v>50</v>
+        <v>52</v>
       </c>
       <c r="K29" s="19" t="s">
-        <v>54</v>
+        <v>56</v>
       </c>
     </row>
     <row r="30" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A30" s="1" t="s">
-        <v>55</v>
+        <v>57</v>
       </c>
       <c r="B30" s="11" t="n">
         <v>7</v>
@@ -4045,21 +4042,21 @@
       <c r="F30" s="17"/>
       <c r="G30" s="18"/>
       <c r="H30" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I30" s="19" t="s">
-        <v>56</v>
+        <v>58</v>
       </c>
       <c r="J30" s="19" t="s">
-        <v>34</v>
+        <v>37</v>
       </c>
       <c r="K30" s="19" t="s">
-        <v>57</v>
+        <v>59</v>
       </c>
     </row>
     <row r="31" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A31" s="1" t="s">
-        <v>58</v>
+        <v>60</v>
       </c>
       <c r="B31" s="11" t="n">
         <v>8</v>
@@ -4074,21 +4071,21 @@
       <c r="F31" s="17"/>
       <c r="G31" s="18"/>
       <c r="H31" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I31" s="19" t="s">
-        <v>60</v>
+        <v>62</v>
       </c>
       <c r="J31" s="19" t="s">
-        <v>61</v>
+        <v>63</v>
       </c>
       <c r="K31" s="19" t="s">
-        <v>62</v>
+        <v>64</v>
       </c>
     </row>
     <row r="32" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A32" s="1" t="s">
-        <v>63</v>
+        <v>65</v>
       </c>
       <c r="B32" s="11" t="n">
         <v>9</v>
@@ -4103,21 +4100,21 @@
       <c r="F32" s="17"/>
       <c r="G32" s="18"/>
       <c r="H32" s="14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I32" s="19" t="s">
-        <v>65</v>
+        <v>67</v>
       </c>
       <c r="J32" s="19" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="K32" s="19" t="s">
-        <v>67</v>
+        <v>69</v>
       </c>
     </row>
     <row r="33" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A33" s="1" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="B33" s="11" t="n">
         <v>10</v>
@@ -4132,19 +4129,19 @@
       <c r="F33" s="17"/>
       <c r="G33" s="18"/>
       <c r="H33" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I33" s="19" t="s">
-        <v>69</v>
+        <v>71</v>
       </c>
       <c r="J33" s="19" t="s">
-        <v>70</v>
+        <v>72</v>
       </c>
       <c r="K33" s="19"/>
     </row>
     <row r="34" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A34" s="1" t="s">
-        <v>71</v>
+        <v>73</v>
       </c>
       <c r="B34" s="11" t="n">
         <v>11</v>
@@ -4159,19 +4156,19 @@
       <c r="F34" s="17"/>
       <c r="G34" s="18"/>
       <c r="H34" s="14" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I34" s="19" t="s">
-        <v>73</v>
+        <v>75</v>
       </c>
       <c r="J34" s="19" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K34" s="19"/>
     </row>
     <row r="35" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A35" s="1" t="s">
-        <v>75</v>
+        <v>77</v>
       </c>
       <c r="B35" s="11" t="n">
         <v>12</v>
@@ -4186,19 +4183,19 @@
       <c r="F35" s="17"/>
       <c r="G35" s="18"/>
       <c r="H35" s="14" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I35" s="19" t="s">
+        <v>78</v>
+      </c>
+      <c r="J35" s="19" t="s">
         <v>76</v>
-      </c>
-      <c r="J35" s="19" t="s">
-        <v>74</v>
       </c>
       <c r="K35" s="19"/>
     </row>
     <row r="36" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A36" s="1" t="s">
-        <v>77</v>
+        <v>79</v>
       </c>
       <c r="B36" s="11" t="n">
         <v>13</v>
@@ -4213,19 +4210,19 @@
       <c r="F36" s="17"/>
       <c r="G36" s="18"/>
       <c r="H36" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I36" s="19" t="s">
-        <v>78</v>
+        <v>80</v>
       </c>
       <c r="J36" s="19" t="s">
-        <v>79</v>
+        <v>81</v>
       </c>
       <c r="K36" s="19"/>
     </row>
     <row r="37" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A37" s="1" t="s">
-        <v>80</v>
+        <v>82</v>
       </c>
       <c r="B37" s="11" t="n">
         <v>14</v>
@@ -4240,19 +4237,19 @@
       <c r="F37" s="17"/>
       <c r="G37" s="18"/>
       <c r="H37" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I37" s="19" t="s">
-        <v>81</v>
+        <v>83</v>
       </c>
       <c r="J37" s="19" t="s">
-        <v>82</v>
+        <v>84</v>
       </c>
       <c r="K37" s="19"/>
     </row>
     <row r="38" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A38" s="1" t="s">
-        <v>83</v>
+        <v>85</v>
       </c>
       <c r="B38" s="11" t="n">
         <v>15</v>
@@ -4267,19 +4264,19 @@
       <c r="F38" s="17"/>
       <c r="G38" s="18"/>
       <c r="H38" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I38" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J38" s="19" t="s">
-        <v>85</v>
+        <v>87</v>
       </c>
       <c r="K38" s="19"/>
     </row>
     <row r="39" s="20" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A39" s="1" t="s">
-        <v>86</v>
+        <v>88</v>
       </c>
       <c r="B39" s="11" t="n">
         <v>16</v>
@@ -4294,21 +4291,21 @@
       <c r="F39" s="17"/>
       <c r="G39" s="18"/>
       <c r="H39" s="14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I39" s="19" t="s">
-        <v>87</v>
+        <v>89</v>
       </c>
       <c r="J39" s="19" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K39" s="19" t="s">
-        <v>89</v>
+        <v>91</v>
       </c>
     </row>
     <row r="40" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A40" s="1" t="s">
-        <v>90</v>
+        <v>92</v>
       </c>
       <c r="B40" s="11" t="n">
         <v>17</v>
@@ -4323,21 +4320,21 @@
       <c r="F40" s="17"/>
       <c r="G40" s="18"/>
       <c r="H40" s="14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I40" s="19" t="s">
-        <v>84</v>
+        <v>86</v>
       </c>
       <c r="J40" s="19" t="s">
-        <v>88</v>
+        <v>90</v>
       </c>
       <c r="K40" s="19" t="s">
-        <v>91</v>
+        <v>93</v>
       </c>
     </row>
     <row r="41" s="20" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A41" s="1" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="B41" s="11" t="n">
         <v>18</v>
@@ -4352,21 +4349,21 @@
       <c r="F41" s="17"/>
       <c r="G41" s="18"/>
       <c r="H41" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I41" s="19" t="s">
-        <v>93</v>
+        <v>95</v>
       </c>
       <c r="J41" s="19" t="s">
-        <v>94</v>
+        <v>96</v>
       </c>
       <c r="K41" s="19" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
     </row>
     <row r="42" s="20" customFormat="true" ht="24" hidden="false" customHeight="true" outlineLevel="0" collapsed="false">
       <c r="A42" s="1" t="s">
-        <v>96</v>
+        <v>98</v>
       </c>
       <c r="B42" s="11" t="n">
         <v>19</v>
@@ -4381,19 +4378,19 @@
       <c r="F42" s="17"/>
       <c r="G42" s="18"/>
       <c r="H42" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I42" s="19" t="s">
-        <v>97</v>
+        <v>99</v>
       </c>
       <c r="J42" s="19" t="s">
-        <v>98</v>
+        <v>100</v>
       </c>
       <c r="K42" s="19"/>
     </row>
     <row r="43" s="20" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A43" s="1" t="s">
-        <v>99</v>
+        <v>101</v>
       </c>
       <c r="B43" s="11" t="n">
         <v>20</v>
@@ -4408,21 +4405,21 @@
       <c r="F43" s="17"/>
       <c r="G43" s="18"/>
       <c r="H43" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I43" s="19" t="s">
-        <v>100</v>
+        <v>102</v>
       </c>
       <c r="J43" s="19" t="s">
-        <v>101</v>
+        <v>103</v>
       </c>
       <c r="K43" s="19" t="s">
-        <v>102</v>
+        <v>104</v>
       </c>
     </row>
     <row r="44" s="20" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A44" s="1" t="s">
-        <v>103</v>
+        <v>105</v>
       </c>
       <c r="B44" s="11" t="n">
         <v>21</v>
@@ -4437,21 +4434,21 @@
       <c r="F44" s="17"/>
       <c r="G44" s="18"/>
       <c r="H44" s="14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I44" s="19" t="s">
-        <v>104</v>
+        <v>106</v>
       </c>
       <c r="J44" s="19" t="s">
-        <v>105</v>
+        <v>107</v>
       </c>
       <c r="K44" s="19" t="s">
-        <v>106</v>
+        <v>108</v>
       </c>
     </row>
     <row r="45" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A45" s="1" t="s">
-        <v>107</v>
+        <v>109</v>
       </c>
       <c r="B45" s="11" t="n">
         <v>22</v>
@@ -4466,21 +4463,21 @@
       <c r="F45" s="17"/>
       <c r="G45" s="18"/>
       <c r="H45" s="14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I45" s="19" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="J45" s="19" t="s">
-        <v>109</v>
+        <v>111</v>
       </c>
       <c r="K45" s="19" t="s">
-        <v>110</v>
+        <v>112</v>
       </c>
     </row>
     <row r="46" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A46" s="1" t="s">
-        <v>111</v>
+        <v>113</v>
       </c>
       <c r="B46" s="11" t="n">
         <v>23</v>
@@ -4493,19 +4490,19 @@
       <c r="F46" s="17"/>
       <c r="G46" s="18"/>
       <c r="H46" s="14" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I46" s="19" t="s">
-        <v>112</v>
+        <v>114</v>
       </c>
       <c r="J46" s="19" t="s">
-        <v>74</v>
+        <v>76</v>
       </c>
       <c r="K46" s="19"/>
     </row>
     <row r="47" s="20" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A47" s="1" t="s">
-        <v>113</v>
+        <v>115</v>
       </c>
       <c r="B47" s="11" t="n">
         <v>24</v>
@@ -4518,19 +4515,19 @@
       <c r="F47" s="17"/>
       <c r="G47" s="18"/>
       <c r="H47" s="14" t="s">
-        <v>72</v>
+        <v>74</v>
       </c>
       <c r="I47" s="19" t="s">
-        <v>114</v>
+        <v>116</v>
       </c>
       <c r="J47" s="19" t="s">
-        <v>115</v>
+        <v>117</v>
       </c>
       <c r="K47" s="19"/>
     </row>
     <row r="48" s="21" customFormat="true" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A48" s="1" t="s">
-        <v>116</v>
+        <v>118</v>
       </c>
       <c r="B48" s="11" t="n">
         <v>25</v>
@@ -4543,19 +4540,19 @@
       <c r="F48" s="17"/>
       <c r="G48" s="18"/>
       <c r="H48" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I48" s="19" t="s">
-        <v>117</v>
+        <v>119</v>
       </c>
       <c r="J48" s="19" t="s">
-        <v>118</v>
+        <v>120</v>
       </c>
       <c r="K48" s="19"/>
     </row>
     <row r="49" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A49" s="1" t="s">
-        <v>119</v>
+        <v>121</v>
       </c>
       <c r="B49" s="11" t="n">
         <v>26</v>
@@ -4568,19 +4565,19 @@
       <c r="F49" s="17"/>
       <c r="G49" s="18"/>
       <c r="H49" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I49" s="19" t="s">
-        <v>120</v>
+        <v>122</v>
       </c>
       <c r="J49" s="19" t="s">
-        <v>121</v>
+        <v>123</v>
       </c>
       <c r="K49" s="19"/>
     </row>
     <row r="50" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A50" s="1" t="s">
-        <v>122</v>
+        <v>124</v>
       </c>
       <c r="B50" s="11" t="n">
         <v>27</v>
@@ -4593,19 +4590,19 @@
       <c r="F50" s="17"/>
       <c r="G50" s="18"/>
       <c r="H50" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I50" s="19" t="s">
-        <v>123</v>
+        <v>125</v>
       </c>
       <c r="J50" s="19" t="s">
-        <v>124</v>
+        <v>126</v>
       </c>
       <c r="K50" s="19"/>
     </row>
     <row r="51" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A51" s="1" t="s">
-        <v>125</v>
+        <v>127</v>
       </c>
       <c r="B51" s="11" t="n">
         <v>28</v>
@@ -4618,19 +4615,19 @@
       <c r="F51" s="17"/>
       <c r="G51" s="18"/>
       <c r="H51" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I51" s="19" t="s">
-        <v>126</v>
+        <v>128</v>
       </c>
       <c r="J51" s="19" t="s">
-        <v>127</v>
+        <v>129</v>
       </c>
       <c r="K51" s="19"/>
     </row>
     <row r="52" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A52" s="1" t="s">
-        <v>128</v>
+        <v>130</v>
       </c>
       <c r="B52" s="11" t="n">
         <v>29</v>
@@ -4643,19 +4640,19 @@
       <c r="F52" s="17"/>
       <c r="G52" s="18"/>
       <c r="H52" s="14" t="s">
-        <v>59</v>
+        <v>61</v>
       </c>
       <c r="I52" s="19" t="s">
-        <v>129</v>
+        <v>131</v>
       </c>
       <c r="J52" s="19" t="s">
-        <v>130</v>
+        <v>132</v>
       </c>
       <c r="K52" s="19"/>
     </row>
     <row r="53" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A53" s="1" t="s">
-        <v>131</v>
+        <v>133</v>
       </c>
       <c r="B53" s="11" t="n">
         <v>30</v>
@@ -4668,21 +4665,21 @@
       <c r="F53" s="17"/>
       <c r="G53" s="18"/>
       <c r="H53" s="14" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="I53" s="19" t="s">
-        <v>132</v>
+        <v>134</v>
       </c>
       <c r="J53" s="19" t="s">
-        <v>133</v>
+        <v>135</v>
       </c>
       <c r="K53" s="19" t="s">
-        <v>134</v>
+        <v>136</v>
       </c>
     </row>
     <row r="54" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A54" s="1" t="s">
-        <v>135</v>
+        <v>137</v>
       </c>
       <c r="B54" s="11" t="n">
         <v>31</v>
@@ -4695,19 +4692,19 @@
       <c r="F54" s="17"/>
       <c r="G54" s="18"/>
       <c r="H54" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I54" s="19" t="s">
-        <v>136</v>
+        <v>138</v>
       </c>
       <c r="J54" s="19" t="s">
-        <v>137</v>
+        <v>139</v>
       </c>
       <c r="K54" s="19"/>
     </row>
     <row r="55" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A55" s="1" t="s">
-        <v>138</v>
+        <v>140</v>
       </c>
       <c r="B55" s="11" t="n">
         <v>32</v>
@@ -4720,19 +4717,19 @@
       <c r="F55" s="17"/>
       <c r="G55" s="18"/>
       <c r="H55" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I55" s="19" t="s">
-        <v>139</v>
+        <v>141</v>
       </c>
       <c r="J55" s="19" t="s">
-        <v>140</v>
+        <v>142</v>
       </c>
       <c r="K55" s="19"/>
     </row>
     <row r="56" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A56" s="1" t="s">
-        <v>141</v>
+        <v>143</v>
       </c>
       <c r="B56" s="11" t="n">
         <v>33</v>
@@ -4745,19 +4742,19 @@
       <c r="F56" s="17"/>
       <c r="G56" s="18"/>
       <c r="H56" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I56" s="19" t="s">
-        <v>142</v>
+        <v>144</v>
       </c>
       <c r="J56" s="19" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="K56" s="19"/>
     </row>
     <row r="57" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A57" s="1" t="s">
-        <v>144</v>
+        <v>146</v>
       </c>
       <c r="B57" s="11" t="n">
         <v>34</v>
@@ -4770,19 +4767,19 @@
       <c r="F57" s="17"/>
       <c r="G57" s="18"/>
       <c r="H57" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I57" s="19" t="s">
+        <v>147</v>
+      </c>
+      <c r="J57" s="19" t="s">
         <v>145</v>
-      </c>
-      <c r="J57" s="19" t="s">
-        <v>143</v>
       </c>
       <c r="K57" s="19"/>
     </row>
     <row r="58" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A58" s="1" t="s">
-        <v>146</v>
+        <v>148</v>
       </c>
       <c r="B58" s="11" t="n">
         <v>35</v>
@@ -4795,19 +4792,19 @@
       <c r="F58" s="17"/>
       <c r="G58" s="18"/>
       <c r="H58" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I58" s="19" t="s">
-        <v>147</v>
+        <v>149</v>
       </c>
       <c r="J58" s="19" t="s">
-        <v>143</v>
+        <v>145</v>
       </c>
       <c r="K58" s="19"/>
     </row>
     <row r="59" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A59" s="1" t="s">
-        <v>148</v>
+        <v>150</v>
       </c>
       <c r="B59" s="11" t="n">
         <v>36</v>
@@ -4820,19 +4817,19 @@
       <c r="F59" s="17"/>
       <c r="G59" s="18"/>
       <c r="H59" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I59" s="19" t="s">
-        <v>149</v>
+        <v>151</v>
       </c>
       <c r="J59" s="19" t="s">
-        <v>150</v>
+        <v>152</v>
       </c>
       <c r="K59" s="19"/>
     </row>
     <row r="60" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A60" s="1" t="s">
-        <v>151</v>
+        <v>153</v>
       </c>
       <c r="B60" s="11" t="n">
         <v>37</v>
@@ -4845,19 +4842,19 @@
       <c r="F60" s="17"/>
       <c r="G60" s="18"/>
       <c r="H60" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I60" s="19" t="s">
-        <v>152</v>
+        <v>154</v>
       </c>
       <c r="J60" s="19" t="s">
-        <v>153</v>
+        <v>155</v>
       </c>
       <c r="K60" s="19"/>
     </row>
     <row r="61" customFormat="false" ht="23.85" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A61" s="1" t="s">
-        <v>154</v>
+        <v>156</v>
       </c>
       <c r="B61" s="11" t="n">
         <v>38</v>
@@ -4870,19 +4867,19 @@
       <c r="F61" s="17"/>
       <c r="G61" s="18"/>
       <c r="H61" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I61" s="19" t="s">
-        <v>155</v>
+        <v>157</v>
       </c>
       <c r="J61" s="19" t="s">
-        <v>156</v>
+        <v>158</v>
       </c>
       <c r="K61" s="19"/>
     </row>
     <row r="62" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A62" s="1" t="s">
-        <v>157</v>
+        <v>159</v>
       </c>
       <c r="B62" s="11" t="n">
         <v>39</v>
@@ -4895,13 +4892,13 @@
       <c r="F62" s="17"/>
       <c r="G62" s="18"/>
       <c r="H62" s="14" t="s">
-        <v>32</v>
+        <v>35</v>
       </c>
       <c r="I62" s="1" t="s">
-        <v>158</v>
+        <v>160</v>
       </c>
       <c r="J62" s="19" t="s">
-        <v>159</v>
+        <v>161</v>
       </c>
       <c r="K62" s="19"/>
     </row>
@@ -5401,11 +5398,11 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="D26" activeCellId="0" sqref="D26"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -5416,7 +5413,7 @@
   <sheetData>
     <row r="1" s="24" customFormat="true" ht="17.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B1" s="22" t="n">
         <v>1</v>
@@ -5429,21 +5426,21 @@
     </row>
     <row r="2" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B2" s="25" t="n">
         <v>44831</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="26" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B3" s="25" t="n">
         <v>44838</v>
@@ -5455,10 +5452,10 @@
     </row>
     <row r="4" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -5476,10 +5473,10 @@
     <row r="6" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="22"/>
       <c r="B6" s="28" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -5487,7 +5484,7 @@
     </row>
     <row r="7" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B7" s="22" t="n">
         <v>4</v>
@@ -5499,7 +5496,7 @@
     </row>
     <row r="8" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B8" s="22" t="n">
         <f aca="false">B7-C8</f>
@@ -5515,7 +5512,7 @@
     </row>
     <row r="9" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B9" s="22" t="n">
         <f aca="false">B8-C9</f>
@@ -5531,7 +5528,7 @@
     </row>
     <row r="10" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B10" s="22" t="n">
         <f aca="false">B9-C10</f>
@@ -5547,7 +5544,7 @@
     </row>
     <row r="11" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B11" s="22" t="n">
         <f aca="false">B10-C11</f>
@@ -5563,7 +5560,7 @@
     </row>
     <row r="12" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B12" s="22" t="n">
         <f aca="false">B11-C12</f>
@@ -5579,15 +5576,15 @@
     </row>
     <row r="13" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B13" s="22" t="n">
         <f aca="false">B12-C13</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C13" s="22" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 6")</f>
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="D13" s="22"/>
       <c r="E13" s="22"/>
@@ -5595,11 +5592,11 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B14" s="22" t="n">
         <f aca="false">B13-C14</f>
-        <v>2</v>
+        <v>0</v>
       </c>
       <c r="C14" s="22" t="n">
         <f aca="false">COUNTIF(E$17:E$995, "Completed Day 7")</f>
@@ -5619,22 +5616,22 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F16" s="29" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5642,13 +5639,13 @@
         <v>1</v>
       </c>
       <c r="B17" s="30" t="s">
-        <v>30</v>
+        <v>33</v>
       </c>
       <c r="D17" s="31" t="s">
-        <v>177</v>
+        <v>179</v>
       </c>
       <c r="E17" s="32" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="18" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5656,13 +5653,13 @@
         <v>2</v>
       </c>
       <c r="B18" s="30" t="s">
-        <v>36</v>
+        <v>39</v>
       </c>
       <c r="D18" s="30" t="s">
-        <v>179</v>
+        <v>181</v>
       </c>
       <c r="E18" s="32" t="s">
-        <v>178</v>
+        <v>180</v>
       </c>
     </row>
     <row r="19" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5670,13 +5667,13 @@
         <v>3</v>
       </c>
       <c r="B19" s="30" t="s">
-        <v>39</v>
+        <v>42</v>
       </c>
       <c r="D19" s="30" t="s">
-        <v>180</v>
+        <v>182</v>
       </c>
       <c r="E19" s="32" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="20" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -5684,30 +5681,42 @@
         <v>4</v>
       </c>
       <c r="B20" s="30" t="s">
-        <v>44</v>
+        <v>46</v>
       </c>
       <c r="D20" s="30" t="s">
-        <v>182</v>
+        <v>184</v>
       </c>
       <c r="E20" s="32" t="s">
-        <v>181</v>
+        <v>183</v>
       </c>
     </row>
     <row r="21" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A21" s="0" t="n">
         <v>5</v>
       </c>
-      <c r="B21" s="30"/>
-      <c r="D21" s="30"/>
-      <c r="E21" s="32"/>
-    </row>
-    <row r="22" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
+      <c r="B21" s="30" t="s">
+        <v>42</v>
+      </c>
+      <c r="D21" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="E21" s="32" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="22" customFormat="false" ht="12.8" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A22" s="0" t="n">
         <v>6</v>
       </c>
-      <c r="B22" s="30"/>
-      <c r="D22" s="30"/>
-      <c r="E22" s="32"/>
+      <c r="B22" s="30" t="s">
+        <v>46</v>
+      </c>
+      <c r="D22" s="30" t="s">
+        <v>185</v>
+      </c>
+      <c r="E22" s="32" t="s">
+        <v>180</v>
+      </c>
     </row>
     <row r="23" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A23" s="0" t="n">
@@ -6378,11 +6387,11 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -6393,7 +6402,7 @@
   <sheetData>
     <row r="1" s="24" customFormat="true" ht="17.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B1" s="22" t="n">
         <f aca="false">'Sprint 01 Backlog'!B1+1</f>
@@ -6407,7 +6416,7 @@
     </row>
     <row r="2" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B2" s="25" t="n">
         <f aca="false">'Sprint 01 Backlog'!B3</f>
@@ -6415,14 +6424,14 @@
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="26" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B3" s="25" t="n">
         <f aca="false">B2+7</f>
@@ -6435,10 +6444,10 @@
     </row>
     <row r="4" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -6456,10 +6465,10 @@
     <row r="6" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="22"/>
       <c r="B6" s="28" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -6467,7 +6476,7 @@
     </row>
     <row r="7" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B7" s="22" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -6480,7 +6489,7 @@
     </row>
     <row r="8" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B8" s="22" t="n">
         <f aca="false">B7-C8</f>
@@ -6496,7 +6505,7 @@
     </row>
     <row r="9" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B9" s="22" t="n">
         <f aca="false">B8-C9</f>
@@ -6512,7 +6521,7 @@
     </row>
     <row r="10" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B10" s="22" t="n">
         <f aca="false">B9-C10</f>
@@ -6528,7 +6537,7 @@
     </row>
     <row r="11" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B11" s="22" t="n">
         <f aca="false">B10-C11</f>
@@ -6544,7 +6553,7 @@
     </row>
     <row r="12" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B12" s="22" t="n">
         <f aca="false">B11-C12</f>
@@ -6560,7 +6569,7 @@
     </row>
     <row r="13" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B13" s="22" t="n">
         <f aca="false">B12-C13</f>
@@ -6576,7 +6585,7 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B14" s="22" t="n">
         <f aca="false">B13-C14</f>
@@ -6600,22 +6609,22 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F16" s="29" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -6624,7 +6633,7 @@
       </c>
       <c r="B17" s="33"/>
       <c r="D17" s="34" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E17" s="35"/>
     </row>
@@ -7341,7 +7350,7 @@
       <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -7352,7 +7361,7 @@
   <sheetData>
     <row r="1" s="24" customFormat="true" ht="17.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B1" s="22" t="n">
         <f aca="false">'Sprint 02 Backlog'!B1+1</f>
@@ -7366,7 +7375,7 @@
     </row>
     <row r="2" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B2" s="25" t="n">
         <f aca="false">'Sprint 02 Backlog'!B3</f>
@@ -7374,14 +7383,14 @@
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="26" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B3" s="25" t="n">
         <f aca="false">B2+7</f>
@@ -7394,10 +7403,10 @@
     </row>
     <row r="4" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -7415,10 +7424,10 @@
     <row r="6" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="22"/>
       <c r="B6" s="28" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -7426,7 +7435,7 @@
     </row>
     <row r="7" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B7" s="22" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -7439,7 +7448,7 @@
     </row>
     <row r="8" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B8" s="22" t="n">
         <f aca="false">B7-C8</f>
@@ -7455,7 +7464,7 @@
     </row>
     <row r="9" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B9" s="22" t="n">
         <f aca="false">B8-C9</f>
@@ -7471,7 +7480,7 @@
     </row>
     <row r="10" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B10" s="22" t="n">
         <f aca="false">B9-C10</f>
@@ -7487,7 +7496,7 @@
     </row>
     <row r="11" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B11" s="22" t="n">
         <f aca="false">B10-C11</f>
@@ -7503,7 +7512,7 @@
     </row>
     <row r="12" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B12" s="22" t="n">
         <f aca="false">B11-C12</f>
@@ -7519,7 +7528,7 @@
     </row>
     <row r="13" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B13" s="22" t="n">
         <f aca="false">B12-C13</f>
@@ -7535,7 +7544,7 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B14" s="22" t="n">
         <f aca="false">B13-C14</f>
@@ -7559,22 +7568,22 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F16" s="29" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -7583,7 +7592,7 @@
       </c>
       <c r="B17" s="33"/>
       <c r="D17" s="34" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E17" s="35"/>
     </row>
@@ -8300,7 +8309,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -8311,7 +8320,7 @@
   <sheetData>
     <row r="1" s="24" customFormat="true" ht="17.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B1" s="22" t="n">
         <f aca="false">'Sprint 03 Backlog'!B1+1</f>
@@ -8325,21 +8334,21 @@
     </row>
     <row r="2" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B2" s="25" t="n">
         <v>44873</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="26" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B3" s="25" t="n">
         <f aca="false">B2+7</f>
@@ -8352,10 +8361,10 @@
     </row>
     <row r="4" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -8373,10 +8382,10 @@
     <row r="6" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="22"/>
       <c r="B6" s="28" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -8384,7 +8393,7 @@
     </row>
     <row r="7" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B7" s="22" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -8397,7 +8406,7 @@
     </row>
     <row r="8" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B8" s="22" t="n">
         <f aca="false">B7-C8</f>
@@ -8413,7 +8422,7 @@
     </row>
     <row r="9" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B9" s="22" t="n">
         <f aca="false">B8-C9</f>
@@ -8429,7 +8438,7 @@
     </row>
     <row r="10" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B10" s="22" t="n">
         <f aca="false">B9-C10</f>
@@ -8445,7 +8454,7 @@
     </row>
     <row r="11" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B11" s="22" t="n">
         <f aca="false">B10-C11</f>
@@ -8461,7 +8470,7 @@
     </row>
     <row r="12" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B12" s="22" t="n">
         <f aca="false">B11-C12</f>
@@ -8477,7 +8486,7 @@
     </row>
     <row r="13" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B13" s="22" t="n">
         <f aca="false">B12-C13</f>
@@ -8493,7 +8502,7 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B14" s="22" t="n">
         <f aca="false">B13-C14</f>
@@ -8517,22 +8526,22 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F16" s="29" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -8541,7 +8550,7 @@
       </c>
       <c r="B17" s="33"/>
       <c r="D17" s="34" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E17" s="35"/>
     </row>
@@ -9258,7 +9267,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -9269,7 +9278,7 @@
   <sheetData>
     <row r="1" s="24" customFormat="true" ht="17.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B1" s="22" t="n">
         <f aca="false">'Sprint 04 Backlog'!B1+1</f>
@@ -9283,7 +9292,7 @@
     </row>
     <row r="2" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B2" s="25" t="n">
         <f aca="false">'Sprint 04 Backlog'!B3</f>
@@ -9291,14 +9300,14 @@
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="26" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B3" s="25" t="n">
         <f aca="false">B2+7</f>
@@ -9311,10 +9320,10 @@
     </row>
     <row r="4" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -9332,10 +9341,10 @@
     <row r="6" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="22"/>
       <c r="B6" s="28" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -9343,7 +9352,7 @@
     </row>
     <row r="7" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B7" s="22" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -9356,7 +9365,7 @@
     </row>
     <row r="8" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B8" s="22" t="n">
         <f aca="false">B7-C8</f>
@@ -9372,7 +9381,7 @@
     </row>
     <row r="9" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B9" s="22" t="n">
         <f aca="false">B8-C9</f>
@@ -9388,7 +9397,7 @@
     </row>
     <row r="10" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B10" s="22" t="n">
         <f aca="false">B9-C10</f>
@@ -9404,7 +9413,7 @@
     </row>
     <row r="11" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B11" s="22" t="n">
         <f aca="false">B10-C11</f>
@@ -9420,7 +9429,7 @@
     </row>
     <row r="12" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B12" s="22" t="n">
         <f aca="false">B11-C12</f>
@@ -9436,7 +9445,7 @@
     </row>
     <row r="13" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B13" s="22" t="n">
         <f aca="false">B12-C13</f>
@@ -9452,7 +9461,7 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B14" s="22" t="n">
         <f aca="false">B13-C14</f>
@@ -9476,22 +9485,22 @@
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F16" s="29" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -9500,7 +9509,7 @@
       </c>
       <c r="B17" s="33"/>
       <c r="D17" s="34" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E17" s="35"/>
     </row>
@@ -10217,7 +10226,7 @@
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -10228,13 +10237,13 @@
   <sheetData>
     <row r="1" s="24" customFormat="true" ht="17.45" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A1" s="22" t="s">
-        <v>8</v>
+        <v>11</v>
       </c>
       <c r="B1" s="22" t="n">
         <v>6</v>
       </c>
       <c r="C1" s="22" t="s">
-        <v>184</v>
+        <v>187</v>
       </c>
       <c r="D1" s="23" t="s">
         <v>2</v>
@@ -10243,21 +10252,21 @@
     </row>
     <row r="2" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A2" s="22" t="s">
-        <v>160</v>
+        <v>162</v>
       </c>
       <c r="B2" s="25" t="n">
         <v>44894</v>
       </c>
       <c r="C2" s="22"/>
       <c r="D2" s="26" t="s">
-        <v>161</v>
+        <v>163</v>
       </c>
       <c r="E2" s="22"/>
       <c r="F2" s="22"/>
     </row>
     <row r="3" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A3" s="22" t="s">
-        <v>162</v>
+        <v>164</v>
       </c>
       <c r="B3" s="25" t="n">
         <f aca="false">B2+7</f>
@@ -10270,10 +10279,10 @@
     </row>
     <row r="4" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A4" s="22" t="s">
-        <v>163</v>
+        <v>165</v>
       </c>
       <c r="B4" s="27" t="s">
-        <v>164</v>
+        <v>166</v>
       </c>
       <c r="C4" s="22"/>
       <c r="D4" s="22"/>
@@ -10291,10 +10300,10 @@
     <row r="6" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A6" s="22"/>
       <c r="B6" s="28" t="s">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="C6" s="22" t="s">
-        <v>165</v>
+        <v>167</v>
       </c>
       <c r="D6" s="22"/>
       <c r="E6" s="22"/>
@@ -10302,7 +10311,7 @@
     </row>
     <row r="7" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A7" s="22" t="s">
-        <v>166</v>
+        <v>168</v>
       </c>
       <c r="B7" s="22" t="n">
         <f aca="false">COUNTA(D17:D995)</f>
@@ -10315,7 +10324,7 @@
     </row>
     <row r="8" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A8" s="22" t="s">
-        <v>167</v>
+        <v>169</v>
       </c>
       <c r="B8" s="22" t="n">
         <f aca="false">B7-C8</f>
@@ -10331,7 +10340,7 @@
     </row>
     <row r="9" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A9" s="22" t="s">
-        <v>168</v>
+        <v>170</v>
       </c>
       <c r="B9" s="22" t="n">
         <f aca="false">B8-C9</f>
@@ -10347,7 +10356,7 @@
     </row>
     <row r="10" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A10" s="22" t="s">
-        <v>169</v>
+        <v>171</v>
       </c>
       <c r="B10" s="22" t="n">
         <f aca="false">B9-C10</f>
@@ -10363,7 +10372,7 @@
     </row>
     <row r="11" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A11" s="22" t="s">
-        <v>170</v>
+        <v>172</v>
       </c>
       <c r="B11" s="22" t="n">
         <f aca="false">B10-C11</f>
@@ -10379,7 +10388,7 @@
     </row>
     <row r="12" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A12" s="22" t="s">
-        <v>171</v>
+        <v>173</v>
       </c>
       <c r="B12" s="22" t="n">
         <f aca="false">B11-C12</f>
@@ -10395,7 +10404,7 @@
     </row>
     <row r="13" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A13" s="22" t="s">
-        <v>172</v>
+        <v>174</v>
       </c>
       <c r="B13" s="22" t="n">
         <f aca="false">B12-C13</f>
@@ -10411,7 +10420,7 @@
     </row>
     <row r="14" s="24" customFormat="true" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A14" s="22" t="s">
-        <v>173</v>
+        <v>175</v>
       </c>
       <c r="B14" s="22" t="n">
         <f aca="false">B13-C14</f>
@@ -10430,29 +10439,29 @@
       <c r="B15" s="22"/>
       <c r="C15" s="22"/>
       <c r="D15" s="22" t="s">
-        <v>185</v>
+        <v>188</v>
       </c>
       <c r="E15" s="22"/>
       <c r="F15" s="22"/>
     </row>
     <row r="16" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
       <c r="A16" s="29" t="s">
-        <v>174</v>
+        <v>176</v>
       </c>
       <c r="B16" s="29" t="s">
-        <v>20</v>
+        <v>23</v>
       </c>
       <c r="C16" s="29" t="s">
-        <v>175</v>
+        <v>177</v>
       </c>
       <c r="D16" s="29" t="s">
-        <v>176</v>
+        <v>178</v>
       </c>
       <c r="E16" s="29" t="s">
-        <v>25</v>
+        <v>28</v>
       </c>
       <c r="F16" s="29" t="s">
-        <v>29</v>
+        <v>32</v>
       </c>
     </row>
     <row r="17" customFormat="false" ht="12.75" hidden="false" customHeight="false" outlineLevel="0" collapsed="false">
@@ -10461,7 +10470,7 @@
       </c>
       <c r="B17" s="33"/>
       <c r="D17" s="34" t="s">
-        <v>183</v>
+        <v>186</v>
       </c>
       <c r="E17" s="35"/>
     </row>

</xml_diff>

<commit_message>
Completed Day 6 Backlog.
</commit_message>
<xml_diff>
--- a/P05/Scrum.xlsx
+++ b/P05/Scrum.xlsx
@@ -5,7 +5,7 @@
   <workbookPr backupFile="false" showObjects="all" date1904="false"/>
   <workbookProtection/>
   <bookViews>
-    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="2"/>
+    <workbookView showHorizontalScroll="true" showVerticalScroll="true" showSheetTabs="true" xWindow="0" yWindow="0" windowWidth="16384" windowHeight="8192" tabRatio="500" firstSheet="0" activeTab="0"/>
   </bookViews>
   <sheets>
     <sheet name="Product Backlog" sheetId="1" state="visible" r:id="rId2"/>
@@ -1030,7 +1030,7 @@
 </styleSheet>
 </file>
 
-<file path=xl/charts/chart15.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1076,10 +1076,10 @@
           <c:layoutTarget val="inner"/>
           <c:xMode val="edge"/>
           <c:yMode val="edge"/>
-          <c:x val="0.0822456753887466"/>
-          <c:y val="0.161896356071113"/>
-          <c:w val="0.884281521263973"/>
-          <c:h val="0.635607111335267"/>
+          <c:x val="0.0822508118910817"/>
+          <c:y val="0.161916771752837"/>
+          <c:w val="0.884211841119161"/>
+          <c:h val="0.635561160151324"/>
         </c:manualLayout>
       </c:layout>
       <c:scatterChart>
@@ -1188,11 +1188,11 @@
           </c:yVal>
           <c:smooth val="0"/>
         </c:ser>
-        <c:axId val="12571629"/>
-        <c:axId val="98322254"/>
+        <c:axId val="95717347"/>
+        <c:axId val="32171240"/>
       </c:scatterChart>
       <c:valAx>
-        <c:axId val="12571629"/>
+        <c:axId val="95717347"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:max val="6"/>
@@ -1259,12 +1259,12 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="98322254"/>
+        <c:crossAx val="32171240"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
       <c:valAx>
-        <c:axId val="98322254"/>
+        <c:axId val="32171240"/>
         <c:scaling>
           <c:orientation val="minMax"/>
           <c:min val="0"/>
@@ -1339,7 +1339,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="12571629"/>
+        <c:crossAx val="95717347"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1366,7 +1366,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart16.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1494,11 +1494,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="75376761"/>
-        <c:axId val="1498183"/>
+        <c:axId val="48815740"/>
+        <c:axId val="77356500"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="75376761"/>
+        <c:axId val="48815740"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1563,7 +1563,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="1498183"/>
+        <c:crossAx val="77356500"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1571,7 +1571,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="1498183"/>
+        <c:axId val="77356500"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1645,7 +1645,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="75376761"/>
+        <c:crossAx val="48815740"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1672,7 +1672,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart17.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -1800,11 +1800,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="43272625"/>
-        <c:axId val="89107661"/>
+        <c:axId val="78112903"/>
+        <c:axId val="53208881"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="43272625"/>
+        <c:axId val="78112903"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1869,7 +1869,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="89107661"/>
+        <c:crossAx val="53208881"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -1877,7 +1877,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="89107661"/>
+        <c:axId val="53208881"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -1951,7 +1951,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="43272625"/>
+        <c:crossAx val="78112903"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -1978,7 +1978,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart18.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2106,11 +2106,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="44556670"/>
-        <c:axId val="29980569"/>
+        <c:axId val="62119034"/>
+        <c:axId val="13294185"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="44556670"/>
+        <c:axId val="62119034"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2175,7 +2175,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="29980569"/>
+        <c:crossAx val="13294185"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2183,7 +2183,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="29980569"/>
+        <c:axId val="13294185"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2257,7 +2257,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="44556670"/>
+        <c:crossAx val="62119034"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2284,7 +2284,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart19.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart5.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2412,11 +2412,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="27674405"/>
-        <c:axId val="74548752"/>
+        <c:axId val="63902839"/>
+        <c:axId val="13627584"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="27674405"/>
+        <c:axId val="63902839"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2481,7 +2481,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="74548752"/>
+        <c:crossAx val="13627584"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2489,7 +2489,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="74548752"/>
+        <c:axId val="13627584"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2563,7 +2563,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="27674405"/>
+        <c:crossAx val="63902839"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2590,7 +2590,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart20.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart6.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -2718,11 +2718,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="57129197"/>
-        <c:axId val="22977046"/>
+        <c:axId val="93622266"/>
+        <c:axId val="77437570"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="57129197"/>
+        <c:axId val="93622266"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2787,7 +2787,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="22977046"/>
+        <c:crossAx val="77437570"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -2795,7 +2795,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="22977046"/>
+        <c:axId val="77437570"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -2869,7 +2869,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="57129197"/>
+        <c:crossAx val="93622266"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -2896,7 +2896,7 @@
 </c:chartSpace>
 </file>
 
-<file path=xl/charts/chart21.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/charts/chart7.xml><?xml version="1.0" encoding="utf-8"?>
 <c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
   <c:lang val="en-US"/>
   <c:roundedCorners val="0"/>
@@ -3024,11 +3024,11 @@
           </c:spPr>
         </c:hiLowLines>
         <c:marker val="0"/>
-        <c:axId val="82518941"/>
-        <c:axId val="77650874"/>
+        <c:axId val="82046388"/>
+        <c:axId val="45614012"/>
       </c:lineChart>
       <c:catAx>
-        <c:axId val="82518941"/>
+        <c:axId val="82046388"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3093,7 +3093,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="77650874"/>
+        <c:crossAx val="45614012"/>
         <c:crosses val="autoZero"/>
         <c:auto val="1"/>
         <c:lblAlgn val="ctr"/>
@@ -3101,7 +3101,7 @@
         <c:noMultiLvlLbl val="0"/>
       </c:catAx>
       <c:valAx>
-        <c:axId val="77650874"/>
+        <c:axId val="45614012"/>
         <c:scaling>
           <c:orientation val="minMax"/>
         </c:scaling>
@@ -3175,7 +3175,7 @@
             </a:pPr>
           </a:p>
         </c:txPr>
-        <c:crossAx val="82518941"/>
+        <c:crossAx val="82046388"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
       </c:valAx>
@@ -3213,9 +3213,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>10</xdr:col>
-      <xdr:colOff>3201480</xdr:colOff>
+      <xdr:colOff>3201120</xdr:colOff>
       <xdr:row>18</xdr:row>
-      <xdr:rowOff>119880</xdr:rowOff>
+      <xdr:rowOff>119520</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3223,8 +3223,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="9115920" y="267840"/>
-        <a:ext cx="5764320" cy="2854800"/>
+        <a:off x="9115200" y="267840"/>
+        <a:ext cx="5763960" cy="2854440"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3248,9 +3248,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3258,8 +3258,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="446400"/>
-        <a:ext cx="3747600" cy="1847520"/>
+        <a:off x="4092120" y="446400"/>
+        <a:ext cx="3746880" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3283,9 +3283,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3293,8 +3293,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="446400"/>
-        <a:ext cx="3747600" cy="1847520"/>
+        <a:off x="4092120" y="446400"/>
+        <a:ext cx="3746880" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3318,9 +3318,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3328,8 +3328,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="446400"/>
-        <a:ext cx="3747600" cy="1847520"/>
+        <a:off x="4092120" y="446400"/>
+        <a:ext cx="3746880" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3353,9 +3353,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3363,8 +3363,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="446400"/>
-        <a:ext cx="3747600" cy="1847520"/>
+        <a:off x="4092120" y="446400"/>
+        <a:ext cx="3746880" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3388,9 +3388,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3398,8 +3398,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="446400"/>
-        <a:ext cx="3747600" cy="1847520"/>
+        <a:off x="4092120" y="446400"/>
+        <a:ext cx="3746880" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3423,9 +3423,9 @@
     </xdr:from>
     <xdr:to>
       <xdr:col>5</xdr:col>
-      <xdr:colOff>518040</xdr:colOff>
+      <xdr:colOff>517680</xdr:colOff>
       <xdr:row>13</xdr:row>
-      <xdr:rowOff>129240</xdr:rowOff>
+      <xdr:rowOff>128880</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame>
       <xdr:nvGraphicFramePr>
@@ -3433,8 +3433,8 @@
         <xdr:cNvGraphicFramePr/>
       </xdr:nvGraphicFramePr>
       <xdr:xfrm>
-        <a:off x="4090680" y="446400"/>
-        <a:ext cx="3747600" cy="1847520"/>
+        <a:off x="4092120" y="446400"/>
+        <a:ext cx="3746880" cy="1847160"/>
       </xdr:xfrm>
       <a:graphic>
         <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
@@ -3455,8 +3455,8 @@
   </sheetPr>
   <dimension ref="A1:K101"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
-      <selection pane="topLeft" activeCell="G14" activeCellId="0" sqref="G14"/>
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A7" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+      <selection pane="topLeft" activeCell="G28" activeCellId="0" sqref="G28"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11.58984375" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
@@ -3466,7 +3466,7 @@
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="1" width="8.57"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="4" min="4" style="1" width="7.41"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="5" min="5" style="1" width="4.43"/>
-    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.41"/>
+    <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="6" min="6" style="1" width="8.4"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="7" min="7" style="1" width="17.71"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="8" min="8" style="1" width="9.59"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="9" min="9" style="1" width="45.57"/>
@@ -3981,7 +3981,9 @@
       <c r="E28" s="11" t="n">
         <v>13</v>
       </c>
-      <c r="F28" s="17"/>
+      <c r="F28" s="17" t="n">
+        <v>2</v>
+      </c>
       <c r="G28" s="18"/>
       <c r="H28" s="14" t="s">
         <v>35</v>
@@ -4010,7 +4012,9 @@
       <c r="E29" s="11" t="n">
         <v>13</v>
       </c>
-      <c r="F29" s="17"/>
+      <c r="F29" s="17" t="n">
+        <v>2</v>
+      </c>
       <c r="G29" s="18"/>
       <c r="H29" s="14" t="s">
         <v>35</v>
@@ -4039,7 +4043,9 @@
       <c r="E30" s="11" t="n">
         <v>5</v>
       </c>
-      <c r="F30" s="17"/>
+      <c r="F30" s="17" t="n">
+        <v>2</v>
+      </c>
       <c r="G30" s="18"/>
       <c r="H30" s="14" t="s">
         <v>35</v>
@@ -4068,7 +4074,9 @@
       <c r="E31" s="11" t="n">
         <v>8</v>
       </c>
-      <c r="F31" s="17"/>
+      <c r="F31" s="17" t="n">
+        <v>2</v>
+      </c>
       <c r="G31" s="18"/>
       <c r="H31" s="14" t="s">
         <v>61</v>
@@ -5402,7 +5410,7 @@
       <selection pane="topLeft" activeCell="D24" activeCellId="0" sqref="D24"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -6387,11 +6395,11 @@
   </sheetPr>
   <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="true" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
+    <sheetView showFormulas="false" showGridLines="true" showRowColHeaders="true" showZeros="true" rightToLeft="false" tabSelected="false" showOutlineSymbols="true" defaultGridColor="true" view="normal" topLeftCell="A1" colorId="64" zoomScale="140" zoomScaleNormal="140" zoomScalePageLayoutView="100" workbookViewId="0">
       <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -7350,7 +7358,7 @@
       <selection pane="topLeft" activeCell="C17" activeCellId="0" sqref="C17"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -8309,7 +8317,7 @@
       <selection pane="topLeft" activeCell="B3" activeCellId="0" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -9267,7 +9275,7 @@
       <selection pane="topLeft" activeCell="B2" activeCellId="0" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>
@@ -10226,7 +10234,7 @@
       <selection pane="topLeft" activeCell="D16" activeCellId="0" sqref="D16"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="11.60546875" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
+  <sheetFormatPr defaultColWidth="11.625" defaultRowHeight="12.75" zeroHeight="false" outlineLevelRow="0" outlineLevelCol="0"/>
   <cols>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="1" min="1" style="0" width="10.29"/>
     <col collapsed="false" customWidth="true" hidden="false" outlineLevel="0" max="3" min="3" style="0" width="12.29"/>

</xml_diff>